<commit_message>
Just a change in an input file
</commit_message>
<xml_diff>
--- a/Input/Envelopes.xlsx
+++ b/Input/Envelopes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20374"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pratenr15640\Desktop\EUReCA\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17838F4C-AA87-47EE-9D77-54DB1E6827AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004B0B76-AB8E-4FCF-BEE4-53D9AF02A809}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="225" windowWidth="17985" windowHeight="10440" tabRatio="823" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9587,21 +9587,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B4A72D35825A314C9EB5C5BDD49EC582" ma:contentTypeVersion="10" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="ab3cfd4ffe88710ffd03436b1addd592">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c0574b82-72ca-428d-96cb-9dbc44012ede" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb55e547d0e393e34c6bbb534eb78df0" ns3:_="">
     <xsd:import namespace="c0574b82-72ca-428d-96cb-9dbc44012ede"/>
@@ -9785,31 +9770,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8F108CF-CFD9-47FB-AD65-C74A1CC8D454}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78A0EADE-0FE4-4B1A-A335-85BC59899BDC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="c0574b82-72ca-428d-96cb-9dbc44012ede"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D81EF3F0-7775-4285-BFE0-18A3A29E794A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9825,4 +9801,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78A0EADE-0FE4-4B1A-A335-85BC59899BDC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="c0574b82-72ca-428d-96cb-9dbc44012ede"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8F108CF-CFD9-47FB-AD65-C74A1CC8D454}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>